<commit_message>
JDBC files have updated
</commit_message>
<xml_diff>
--- a/src/test/java/apachePOI/resource/ScenarioResults.xlsx
+++ b/src/test/java/apachePOI/resource/ScenarioResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="5">
   <si>
     <t>Create and Delete CitizenShip From Excel</t>
   </si>
@@ -21,6 +21,12 @@
   </si>
   <si>
     <t>chrome</t>
+  </si>
+  <si>
+    <t>States testing with JDBC</t>
+  </si>
+  <si>
+    <t>FAILED</t>
   </si>
 </sst>
 </file>
@@ -65,7 +71,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -82,6 +88,72 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
The repository has been updated
</commit_message>
<xml_diff>
--- a/src/test/java/apachePOI/resource/ScenarioResults.xlsx
+++ b/src/test/java/apachePOI/resource/ScenarioResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="8">
   <si>
     <t>Create and Delete CitizenShip From Excel</t>
   </si>
@@ -80,7 +80,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -273,6 +273,50 @@
         <v>2</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
The framework has been updated
</commit_message>
<xml_diff>
--- a/src/test/java/apachePOI/resource/ScenarioResults.xlsx
+++ b/src/test/java/apachePOI/resource/ScenarioResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="20">
   <si>
     <t>Create and Delete CitizenShip From Excel</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>Create Nationality</t>
+  </si>
+  <si>
+    <t>Create Inventory and Delete</t>
+  </si>
+  <si>
+    <t>UNDEFINED</t>
   </si>
 </sst>
 </file>
@@ -110,7 +116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:C127"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1177,6 +1183,334 @@
         <v>2</v>
       </c>
     </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>16</v>
+      </c>
+      <c r="B98" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>16</v>
+      </c>
+      <c r="B99" t="s">
+        <v>1</v>
+      </c>
+      <c r="C99" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>16</v>
+      </c>
+      <c r="B100" t="s">
+        <v>1</v>
+      </c>
+      <c r="C100" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>16</v>
+      </c>
+      <c r="B101" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>16</v>
+      </c>
+      <c r="B102" t="s">
+        <v>1</v>
+      </c>
+      <c r="C102" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>16</v>
+      </c>
+      <c r="B103" t="s">
+        <v>1</v>
+      </c>
+      <c r="C103" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>16</v>
+      </c>
+      <c r="B104" t="s">
+        <v>1</v>
+      </c>
+      <c r="C104" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>16</v>
+      </c>
+      <c r="B105" t="s">
+        <v>1</v>
+      </c>
+      <c r="C105" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>8</v>
+      </c>
+      <c r="B106" t="s">
+        <v>1</v>
+      </c>
+      <c r="C106" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>8</v>
+      </c>
+      <c r="B107" t="s">
+        <v>1</v>
+      </c>
+      <c r="C107" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>12</v>
+      </c>
+      <c r="B108" t="s">
+        <v>4</v>
+      </c>
+      <c r="C108" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>12</v>
+      </c>
+      <c r="B109" t="s">
+        <v>4</v>
+      </c>
+      <c r="C109" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>18</v>
+      </c>
+      <c r="B110" t="s">
+        <v>19</v>
+      </c>
+      <c r="C110"/>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>18</v>
+      </c>
+      <c r="B111" t="s">
+        <v>4</v>
+      </c>
+      <c r="C111" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>18</v>
+      </c>
+      <c r="B112" t="s">
+        <v>4</v>
+      </c>
+      <c r="C112" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>18</v>
+      </c>
+      <c r="B113" t="s">
+        <v>4</v>
+      </c>
+      <c r="C113" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s">
+        <v>18</v>
+      </c>
+      <c r="B114" t="s">
+        <v>4</v>
+      </c>
+      <c r="C114" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s">
+        <v>18</v>
+      </c>
+      <c r="B115" t="s">
+        <v>4</v>
+      </c>
+      <c r="C115" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s">
+        <v>18</v>
+      </c>
+      <c r="B116" t="s">
+        <v>4</v>
+      </c>
+      <c r="C116" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s">
+        <v>18</v>
+      </c>
+      <c r="B117" t="s">
+        <v>4</v>
+      </c>
+      <c r="C117" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s">
+        <v>18</v>
+      </c>
+      <c r="B118" t="s">
+        <v>4</v>
+      </c>
+      <c r="C118" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s">
+        <v>18</v>
+      </c>
+      <c r="B119" t="s">
+        <v>1</v>
+      </c>
+      <c r="C119" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s">
+        <v>18</v>
+      </c>
+      <c r="B120" t="s">
+        <v>4</v>
+      </c>
+      <c r="C120" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s">
+        <v>18</v>
+      </c>
+      <c r="B121" t="s">
+        <v>4</v>
+      </c>
+      <c r="C121" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>18</v>
+      </c>
+      <c r="B122" t="s">
+        <v>4</v>
+      </c>
+      <c r="C122" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>18</v>
+      </c>
+      <c r="B123" t="s">
+        <v>1</v>
+      </c>
+      <c r="C123" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>18</v>
+      </c>
+      <c r="B124" t="s">
+        <v>1</v>
+      </c>
+      <c r="C124" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>18</v>
+      </c>
+      <c r="B125" t="s">
+        <v>1</v>
+      </c>
+      <c r="C125" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>18</v>
+      </c>
+      <c r="B126" t="s">
+        <v>1</v>
+      </c>
+      <c r="C126" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>18</v>
+      </c>
+      <c r="B127" t="s">
+        <v>1</v>
+      </c>
+      <c r="C127" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
The project has been updated
</commit_message>
<xml_diff>
--- a/src/test/java/apachePOI/resource/ScenarioResults.xlsx
+++ b/src/test/java/apachePOI/resource/ScenarioResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="22">
   <si>
     <t>Create and Delete CitizenShip From Excel</t>
   </si>
@@ -76,6 +76,9 @@
   <si>
     <t>Create Country</t>
   </si>
+  <si>
+    <t>Create CitizenShip and Delete</t>
+  </si>
 </sst>
 </file>
 
@@ -119,7 +122,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C187"/>
+  <dimension ref="A1:C207"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -2174,6 +2177,226 @@
         <v>2</v>
       </c>
     </row>
+    <row r="188">
+      <c r="A188" t="s">
+        <v>3</v>
+      </c>
+      <c r="B188" t="s">
+        <v>1</v>
+      </c>
+      <c r="C188" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="s">
+        <v>3</v>
+      </c>
+      <c r="B189" t="s">
+        <v>1</v>
+      </c>
+      <c r="C189" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="s">
+        <v>21</v>
+      </c>
+      <c r="B190" t="s">
+        <v>4</v>
+      </c>
+      <c r="C190" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="s">
+        <v>21</v>
+      </c>
+      <c r="B191" t="s">
+        <v>4</v>
+      </c>
+      <c r="C191" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="s">
+        <v>21</v>
+      </c>
+      <c r="B192" t="s">
+        <v>4</v>
+      </c>
+      <c r="C192" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="s">
+        <v>21</v>
+      </c>
+      <c r="B193" t="s">
+        <v>4</v>
+      </c>
+      <c r="C193" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="s">
+        <v>21</v>
+      </c>
+      <c r="B194" t="s">
+        <v>4</v>
+      </c>
+      <c r="C194" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="s">
+        <v>21</v>
+      </c>
+      <c r="B195" t="s">
+        <v>4</v>
+      </c>
+      <c r="C195" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="s">
+        <v>21</v>
+      </c>
+      <c r="B196" t="s">
+        <v>4</v>
+      </c>
+      <c r="C196" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="s">
+        <v>21</v>
+      </c>
+      <c r="B197" t="s">
+        <v>4</v>
+      </c>
+      <c r="C197" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="s">
+        <v>21</v>
+      </c>
+      <c r="B198" t="s">
+        <v>4</v>
+      </c>
+      <c r="C198" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="s">
+        <v>21</v>
+      </c>
+      <c r="B199" t="s">
+        <v>4</v>
+      </c>
+      <c r="C199" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="s">
+        <v>21</v>
+      </c>
+      <c r="B200" t="s">
+        <v>4</v>
+      </c>
+      <c r="C200" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="s">
+        <v>21</v>
+      </c>
+      <c r="B201" t="s">
+        <v>4</v>
+      </c>
+      <c r="C201" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="s">
+        <v>21</v>
+      </c>
+      <c r="B202" t="s">
+        <v>4</v>
+      </c>
+      <c r="C202" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="s">
+        <v>21</v>
+      </c>
+      <c r="B203" t="s">
+        <v>1</v>
+      </c>
+      <c r="C203" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="s">
+        <v>21</v>
+      </c>
+      <c r="B204" t="s">
+        <v>1</v>
+      </c>
+      <c r="C204" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="s">
+        <v>21</v>
+      </c>
+      <c r="B205" t="s">
+        <v>1</v>
+      </c>
+      <c r="C205" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="s">
+        <v>21</v>
+      </c>
+      <c r="B206" t="s">
+        <v>1</v>
+      </c>
+      <c r="C206" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="s">
+        <v>21</v>
+      </c>
+      <c r="B207" t="s">
+        <v>1</v>
+      </c>
+      <c r="C207" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>